<commit_message>
Mais tweets & melhorias no código
</commit_message>
<xml_diff>
--- a/League of Legends_1.xlsx
+++ b/League of Legends_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucius\Documents\Insper\s2_2021.1\CDados\Projeto 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F031CA1-D548-4953-8567-99606D8786D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA1D758-4C99-44AD-9C54-2FFBE6B4A05C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="503">
-  <si>
-    <t>Treinamento</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="502">
   <si>
     <t>@aakkari @furia tem um champ no league of legends que se chama akali. sempre que vejo seu @ eu leio akali. é impossível não lembrar da akali. já tô até começando a acostumar que seu nome é akali e não akkari. enfim, desabafei é isso 🙃</t>
   </si>
@@ -1039,9 +1036,6 @@
     <t>mulheres estou jogando league of legends</t>
   </si>
   <si>
-    <t>Teste</t>
-  </si>
-  <si>
     <t>uma call do supermercado vendo anime e a outra jogando league of legends 🤮https://t.co/orgrac6xbp</t>
   </si>
   <si>
@@ -1737,6 +1731,9 @@
   </si>
   <si>
     <t>Relevancia</t>
+  </si>
+  <si>
+    <t>Tweets</t>
   </si>
 </sst>
 </file>
@@ -2163,8 +2160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I301"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2175,15 +2172,15 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>501</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2191,7 +2188,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -2199,7 +2196,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2207,7 +2204,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2215,7 +2212,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2223,7 +2220,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -2231,7 +2228,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -2239,7 +2236,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2247,7 +2244,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2256,7 +2253,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2264,7 +2261,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -2272,7 +2269,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2280,7 +2277,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2288,7 +2285,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -2296,7 +2293,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -2304,7 +2301,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -2312,7 +2309,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -2320,7 +2317,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -2328,7 +2325,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -2336,7 +2333,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -2344,7 +2341,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -2352,7 +2349,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -2360,7 +2357,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -2368,7 +2365,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -2376,7 +2373,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -2384,7 +2381,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -2392,7 +2389,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -2400,7 +2397,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -2408,7 +2405,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -2416,7 +2413,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -2424,7 +2421,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -2432,7 +2429,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -2440,7 +2437,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -2448,7 +2445,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -2456,7 +2453,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -2464,7 +2461,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -2472,7 +2469,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -2480,7 +2477,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -2488,7 +2485,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -2496,7 +2493,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -2504,7 +2501,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -2512,7 +2509,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -2520,7 +2517,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -2528,7 +2525,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -2536,7 +2533,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -2544,7 +2541,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -2552,7 +2549,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -2560,7 +2557,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -2568,7 +2565,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -2576,7 +2573,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -2584,7 +2581,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -2592,7 +2589,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -2600,7 +2597,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -2608,7 +2605,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -2616,7 +2613,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -2624,7 +2621,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57">
         <v>1</v>
@@ -2632,7 +2629,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -2640,7 +2637,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -2648,7 +2645,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -2656,7 +2653,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -2664,7 +2661,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -2672,7 +2669,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -2680,7 +2677,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -2688,7 +2685,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -2696,7 +2693,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -2704,7 +2701,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -2712,7 +2709,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -2720,7 +2717,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -2728,7 +2725,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B70">
         <v>0</v>
@@ -2736,7 +2733,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B71">
         <v>1</v>
@@ -2744,7 +2741,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -2752,7 +2749,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -2760,7 +2757,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B74">
         <v>0</v>
@@ -2768,7 +2765,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -2776,7 +2773,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -2784,7 +2781,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -2792,7 +2789,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B78">
         <v>1</v>
@@ -2800,7 +2797,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -2808,7 +2805,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B80">
         <v>1</v>
@@ -2816,7 +2813,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B81">
         <v>1</v>
@@ -2824,7 +2821,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -2832,7 +2829,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B83">
         <v>1</v>
@@ -2840,7 +2837,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -2848,7 +2845,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -2856,7 +2853,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -2864,7 +2861,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -2872,7 +2869,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -2880,7 +2877,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B89">
         <v>1</v>
@@ -2888,7 +2885,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B90">
         <v>1</v>
@@ -2896,7 +2893,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B91">
         <v>1</v>
@@ -2904,7 +2901,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B92">
         <v>1</v>
@@ -2912,7 +2909,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B93">
         <v>1</v>
@@ -2920,7 +2917,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -2928,7 +2925,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -2936,7 +2933,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B96">
         <v>1</v>
@@ -2944,7 +2941,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B97">
         <v>1</v>
@@ -2952,7 +2949,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B98">
         <v>1</v>
@@ -2960,7 +2957,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -2968,7 +2965,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B100">
         <v>1</v>
@@ -2976,7 +2973,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B101">
         <v>0</v>
@@ -2984,7 +2981,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B102">
         <v>0</v>
@@ -2992,7 +2989,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B103">
         <v>1</v>
@@ -3000,7 +2997,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B104">
         <v>0</v>
@@ -3008,7 +3005,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B105">
         <v>0</v>
@@ -3016,7 +3013,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B106">
         <v>1</v>
@@ -3024,7 +3021,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B107">
         <v>1</v>
@@ -3032,7 +3029,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B108">
         <v>1</v>
@@ -3040,7 +3037,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B109">
         <v>0</v>
@@ -3048,7 +3045,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B110">
         <v>0</v>
@@ -3056,7 +3053,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B111">
         <v>1</v>
@@ -3064,7 +3061,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B112">
         <v>1</v>
@@ -3072,7 +3069,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B113">
         <v>0</v>
@@ -3080,7 +3077,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B114">
         <v>1</v>
@@ -3088,7 +3085,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B115">
         <v>1</v>
@@ -3096,7 +3093,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B116">
         <v>1</v>
@@ -3104,7 +3101,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B117">
         <v>0</v>
@@ -3112,7 +3109,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B118">
         <v>0</v>
@@ -3120,7 +3117,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B119">
         <v>0</v>
@@ -3128,7 +3125,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B120">
         <v>1</v>
@@ -3136,7 +3133,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B121">
         <v>1</v>
@@ -3144,7 +3141,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B122">
         <v>1</v>
@@ -3152,7 +3149,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B123">
         <v>1</v>
@@ -3160,7 +3157,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B124">
         <v>1</v>
@@ -3168,7 +3165,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B125">
         <v>1</v>
@@ -3176,7 +3173,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B126">
         <v>1</v>
@@ -3184,7 +3181,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B127">
         <v>1</v>
@@ -3192,7 +3189,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B128">
         <v>1</v>
@@ -3200,7 +3197,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B129">
         <v>0</v>
@@ -3208,7 +3205,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B130">
         <v>1</v>
@@ -3216,7 +3213,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B131">
         <v>1</v>
@@ -3224,7 +3221,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B132">
         <v>1</v>
@@ -3232,7 +3229,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B133">
         <v>1</v>
@@ -3240,7 +3237,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B134">
         <v>1</v>
@@ -3248,7 +3245,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B135">
         <v>0</v>
@@ -3256,7 +3253,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B136">
         <v>1</v>
@@ -3264,7 +3261,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B137">
         <v>0</v>
@@ -3272,7 +3269,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B138">
         <v>0</v>
@@ -3280,7 +3277,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B139">
         <v>0</v>
@@ -3288,7 +3285,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B140">
         <v>0</v>
@@ -3296,7 +3293,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B141">
         <v>0</v>
@@ -3304,7 +3301,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B142">
         <v>0</v>
@@ -3312,7 +3309,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B143">
         <v>0</v>
@@ -3320,7 +3317,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B144">
         <v>0</v>
@@ -3328,7 +3325,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B145">
         <v>0</v>
@@ -3336,7 +3333,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B146">
         <v>1</v>
@@ -3344,7 +3341,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B147">
         <v>0</v>
@@ -3352,7 +3349,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B148">
         <v>0</v>
@@ -3360,7 +3357,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B149">
         <v>0</v>
@@ -3368,7 +3365,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B150">
         <v>0</v>
@@ -3376,7 +3373,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B151">
         <v>0</v>
@@ -3384,7 +3381,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B152">
         <v>0</v>
@@ -3392,7 +3389,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B153">
         <v>0</v>
@@ -3400,7 +3397,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B154">
         <v>1</v>
@@ -3408,7 +3405,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B155">
         <v>0</v>
@@ -3416,7 +3413,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B156">
         <v>0</v>
@@ -3424,7 +3421,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B157">
         <v>0</v>
@@ -3432,7 +3429,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B158">
         <v>0</v>
@@ -3440,7 +3437,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B159">
         <v>0</v>
@@ -3448,7 +3445,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B160">
         <v>0</v>
@@ -3456,7 +3453,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B161">
         <v>0</v>
@@ -3464,7 +3461,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B162">
         <v>0</v>
@@ -3472,7 +3469,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B163">
         <v>0</v>
@@ -3480,7 +3477,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B164">
         <v>0</v>
@@ -3488,7 +3485,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B165">
         <v>0</v>
@@ -3496,7 +3493,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B166">
         <v>0</v>
@@ -3504,7 +3501,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B167">
         <v>0</v>
@@ -3512,7 +3509,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B168">
         <v>1</v>
@@ -3520,7 +3517,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B169">
         <v>0</v>
@@ -3528,7 +3525,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B170">
         <v>0</v>
@@ -3536,7 +3533,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B171">
         <v>0</v>
@@ -3544,7 +3541,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B172">
         <v>1</v>
@@ -3552,7 +3549,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B173">
         <v>0</v>
@@ -3560,7 +3557,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B174">
         <v>0</v>
@@ -3568,7 +3565,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B175">
         <v>0</v>
@@ -3576,7 +3573,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B176">
         <v>0</v>
@@ -3584,7 +3581,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B177">
         <v>0</v>
@@ -3592,7 +3589,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B178">
         <v>0</v>
@@ -3600,7 +3597,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B179">
         <v>0</v>
@@ -3608,7 +3605,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B180">
         <v>1</v>
@@ -3616,7 +3613,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B181">
         <v>0</v>
@@ -3624,7 +3621,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B182">
         <v>0</v>
@@ -3632,7 +3629,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B183">
         <v>0</v>
@@ -3640,7 +3637,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B184">
         <v>1</v>
@@ -3648,7 +3645,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B185">
         <v>0</v>
@@ -3656,7 +3653,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B186">
         <v>0</v>
@@ -3664,7 +3661,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B187">
         <v>0</v>
@@ -3672,7 +3669,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B188">
         <v>0</v>
@@ -3680,7 +3677,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B189">
         <v>1</v>
@@ -3688,7 +3685,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B190">
         <v>1</v>
@@ -3696,7 +3693,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B191">
         <v>0</v>
@@ -3704,7 +3701,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B192">
         <v>1</v>
@@ -3712,7 +3709,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B193">
         <v>1</v>
@@ -3720,7 +3717,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B194">
         <v>1</v>
@@ -3728,7 +3725,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B195">
         <v>1</v>
@@ -3736,7 +3733,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B196">
         <v>1</v>
@@ -3744,7 +3741,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B197">
         <v>0</v>
@@ -3752,7 +3749,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B198">
         <v>1</v>
@@ -3760,7 +3757,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B199">
         <v>0</v>
@@ -3768,7 +3765,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B200">
         <v>0</v>
@@ -3776,7 +3773,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B201">
         <v>0</v>
@@ -3784,7 +3781,7 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B202">
         <v>0</v>
@@ -3792,7 +3789,7 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B203">
         <v>0</v>
@@ -3800,7 +3797,7 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B204">
         <v>1</v>
@@ -3808,7 +3805,7 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B205">
         <v>1</v>
@@ -3816,7 +3813,7 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B206">
         <v>1</v>
@@ -3824,7 +3821,7 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B207">
         <v>1</v>
@@ -3832,7 +3829,7 @@
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B208">
         <v>1</v>
@@ -3840,7 +3837,7 @@
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B209">
         <v>0</v>
@@ -3848,7 +3845,7 @@
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B210">
         <v>1</v>
@@ -3856,7 +3853,7 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B211">
         <v>0</v>
@@ -3864,7 +3861,7 @@
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B212">
         <v>0</v>
@@ -3872,7 +3869,7 @@
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B213">
         <v>0</v>
@@ -3880,7 +3877,7 @@
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B214">
         <v>1</v>
@@ -3888,7 +3885,7 @@
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B215">
         <v>1</v>
@@ -3896,7 +3893,7 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B216">
         <v>0</v>
@@ -3904,7 +3901,7 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B217">
         <v>1</v>
@@ -3912,7 +3909,7 @@
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B218">
         <v>0</v>
@@ -3920,7 +3917,7 @@
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B219">
         <v>0</v>
@@ -3928,7 +3925,7 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B220">
         <v>1</v>
@@ -3936,7 +3933,7 @@
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B221">
         <v>0</v>
@@ -3944,7 +3941,7 @@
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B222">
         <v>1</v>
@@ -3952,7 +3949,7 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B223">
         <v>1</v>
@@ -3960,7 +3957,7 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B224">
         <v>0</v>
@@ -3968,7 +3965,7 @@
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B225">
         <v>1</v>
@@ -3976,7 +3973,7 @@
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B226">
         <v>0</v>
@@ -3984,7 +3981,7 @@
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B227">
         <v>1</v>
@@ -3992,7 +3989,7 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B228">
         <v>1</v>
@@ -4000,7 +3997,7 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B229">
         <v>0</v>
@@ -4008,7 +4005,7 @@
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B230">
         <v>0</v>
@@ -4016,7 +4013,7 @@
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B231">
         <v>0</v>
@@ -4024,7 +4021,7 @@
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B232">
         <v>1</v>
@@ -4032,7 +4029,7 @@
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B233">
         <v>0</v>
@@ -4040,7 +4037,7 @@
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B234">
         <v>0</v>
@@ -4048,7 +4045,7 @@
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B235">
         <v>0</v>
@@ -4056,7 +4053,7 @@
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B236">
         <v>1</v>
@@ -4064,7 +4061,7 @@
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B237">
         <v>0</v>
@@ -4072,7 +4069,7 @@
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B238">
         <v>0</v>
@@ -4080,7 +4077,7 @@
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B239">
         <v>0</v>
@@ -4088,7 +4085,7 @@
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B240">
         <v>0</v>
@@ -4096,7 +4093,7 @@
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B241">
         <v>1</v>
@@ -4104,7 +4101,7 @@
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B242">
         <v>1</v>
@@ -4112,7 +4109,7 @@
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B243">
         <v>0</v>
@@ -4120,7 +4117,7 @@
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B244">
         <v>1</v>
@@ -4128,7 +4125,7 @@
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B245">
         <v>0</v>
@@ -4136,7 +4133,7 @@
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B246">
         <v>1</v>
@@ -4144,7 +4141,7 @@
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B247">
         <v>1</v>
@@ -4152,7 +4149,7 @@
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B248">
         <v>0</v>
@@ -4160,7 +4157,7 @@
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B249">
         <v>0</v>
@@ -4168,7 +4165,7 @@
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B250">
         <v>0</v>
@@ -4176,7 +4173,7 @@
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B251">
         <v>1</v>
@@ -4184,7 +4181,7 @@
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B252">
         <v>0</v>
@@ -4192,7 +4189,7 @@
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B253">
         <v>1</v>
@@ -4200,7 +4197,7 @@
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B254">
         <v>1</v>
@@ -4208,7 +4205,7 @@
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B255">
         <v>1</v>
@@ -4216,7 +4213,7 @@
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B256">
         <v>0</v>
@@ -4224,7 +4221,7 @@
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B257">
         <v>0</v>
@@ -4232,7 +4229,7 @@
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B258">
         <v>1</v>
@@ -4240,7 +4237,7 @@
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B259">
         <v>0</v>
@@ -4248,7 +4245,7 @@
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B260">
         <v>0</v>
@@ -4256,7 +4253,7 @@
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B261">
         <v>0</v>
@@ -4264,7 +4261,7 @@
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B262">
         <v>0</v>
@@ -4272,7 +4269,7 @@
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B263">
         <v>0</v>
@@ -4280,7 +4277,7 @@
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B264">
         <v>1</v>
@@ -4288,7 +4285,7 @@
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B265">
         <v>0</v>
@@ -4296,7 +4293,7 @@
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B266">
         <v>0</v>
@@ -4304,7 +4301,7 @@
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B267">
         <v>1</v>
@@ -4312,7 +4309,7 @@
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B268">
         <v>0</v>
@@ -4320,7 +4317,7 @@
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B269">
         <v>1</v>
@@ -4328,7 +4325,7 @@
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B270">
         <v>0</v>
@@ -4336,7 +4333,7 @@
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B271">
         <v>1</v>
@@ -4344,7 +4341,7 @@
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B272">
         <v>0</v>
@@ -4352,7 +4349,7 @@
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B273">
         <v>0</v>
@@ -4360,7 +4357,7 @@
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B274">
         <v>1</v>
@@ -4368,7 +4365,7 @@
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B275">
         <v>1</v>
@@ -4376,7 +4373,7 @@
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B276">
         <v>1</v>
@@ -4384,7 +4381,7 @@
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B277">
         <v>0</v>
@@ -4392,7 +4389,7 @@
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B278">
         <v>0</v>
@@ -4400,7 +4397,7 @@
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B279">
         <v>0</v>
@@ -4408,7 +4405,7 @@
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B280">
         <v>1</v>
@@ -4416,7 +4413,7 @@
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B281">
         <v>1</v>
@@ -4424,7 +4421,7 @@
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B282">
         <v>0</v>
@@ -4432,7 +4429,7 @@
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B283">
         <v>0</v>
@@ -4440,7 +4437,7 @@
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B284">
         <v>1</v>
@@ -4448,7 +4445,7 @@
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B285">
         <v>0</v>
@@ -4456,7 +4453,7 @@
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B286">
         <v>1</v>
@@ -4464,7 +4461,7 @@
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B287">
         <v>1</v>
@@ -4472,7 +4469,7 @@
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B288">
         <v>0</v>
@@ -4480,7 +4477,7 @@
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B289">
         <v>0</v>
@@ -4488,7 +4485,7 @@
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B290">
         <v>1</v>
@@ -4496,7 +4493,7 @@
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B291">
         <v>0</v>
@@ -4504,7 +4501,7 @@
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B292">
         <v>0</v>
@@ -4512,7 +4509,7 @@
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B293">
         <v>0</v>
@@ -4520,7 +4517,7 @@
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B294">
         <v>0</v>
@@ -4528,7 +4525,7 @@
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B295">
         <v>1</v>
@@ -4536,7 +4533,7 @@
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B296">
         <v>0</v>
@@ -4544,7 +4541,7 @@
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B297">
         <v>1</v>
@@ -4552,7 +4549,7 @@
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B298">
         <v>1</v>
@@ -4560,7 +4557,7 @@
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B299">
         <v>1</v>
@@ -4568,7 +4565,7 @@
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B300">
         <v>1</v>
@@ -4576,7 +4573,7 @@
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B301">
         <v>0</v>
@@ -4594,9 +4591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4606,15 +4601,15 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>301</v>
+        <v>501</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -4622,7 +4617,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4630,7 +4625,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -4638,7 +4633,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4647,7 +4642,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -4655,7 +4650,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -4663,7 +4658,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -4671,7 +4666,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -4679,7 +4674,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -4687,7 +4682,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -4695,7 +4690,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -4703,7 +4698,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -4711,7 +4706,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -4719,7 +4714,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4727,7 +4722,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -4736,7 +4731,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -4744,7 +4739,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -4752,7 +4747,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -4760,7 +4755,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -4768,7 +4763,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -4776,7 +4771,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -4784,7 +4779,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -4792,7 +4787,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -4800,7 +4795,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -4808,7 +4803,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -4816,7 +4811,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -4824,7 +4819,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -4832,7 +4827,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -4840,7 +4835,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -4848,7 +4843,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -4856,7 +4851,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -4864,7 +4859,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -4872,7 +4867,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -4880,7 +4875,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -4888,7 +4883,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -4896,7 +4891,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -4904,7 +4899,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -4912,7 +4907,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -4920,7 +4915,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -4928,7 +4923,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -4936,7 +4931,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -4944,7 +4939,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -4952,7 +4947,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -4960,7 +4955,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -4968,7 +4963,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -4976,7 +4971,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -4984,7 +4979,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -4992,7 +4987,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -5000,7 +4995,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -5008,7 +5003,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -5016,7 +5011,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -5024,7 +5019,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -5032,7 +5027,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -5040,7 +5035,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -5048,7 +5043,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -5056,7 +5051,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -5064,7 +5059,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -5072,7 +5067,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B59">
         <v>0</v>
@@ -5080,7 +5075,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -5088,7 +5083,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -5096,7 +5091,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -5104,7 +5099,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -5112,7 +5107,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -5120,7 +5115,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -5128,7 +5123,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -5136,7 +5131,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -5144,7 +5139,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -5152,7 +5147,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -5160,7 +5155,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -5168,7 +5163,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -5176,7 +5171,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -5184,7 +5179,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -5192,7 +5187,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -5200,7 +5195,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -5208,7 +5203,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -5216,7 +5211,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -5224,7 +5219,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -5232,7 +5227,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B79">
         <v>1</v>
@@ -5240,7 +5235,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -5248,7 +5243,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -5256,7 +5251,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -5264,7 +5259,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -5272,7 +5267,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -5280,7 +5275,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -5288,7 +5283,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -5296,7 +5291,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -5304,7 +5299,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -5312,7 +5307,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -5320,7 +5315,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -5328,7 +5323,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -5336,7 +5331,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B92">
         <v>1</v>
@@ -5344,7 +5339,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -5352,7 +5347,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -5360,7 +5355,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -5368,7 +5363,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -5376,7 +5371,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B97">
         <v>1</v>
@@ -5384,7 +5379,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B98">
         <v>0</v>
@@ -5392,7 +5387,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -5400,7 +5395,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B100">
         <v>1</v>
@@ -5408,7 +5403,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B101">
         <v>1</v>
@@ -5416,7 +5411,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B102">
         <v>0</v>
@@ -5424,7 +5419,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B103">
         <v>1</v>
@@ -5432,7 +5427,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B104">
         <v>1</v>
@@ -5440,7 +5435,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B105">
         <v>1</v>
@@ -5448,7 +5443,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B106">
         <v>1</v>
@@ -5456,7 +5451,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B107">
         <v>1</v>
@@ -5464,7 +5459,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B108">
         <v>1</v>
@@ -5472,7 +5467,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B109">
         <v>1</v>
@@ -5480,7 +5475,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B110">
         <v>0</v>
@@ -5488,7 +5483,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B111">
         <v>1</v>
@@ -5496,7 +5491,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B112">
         <v>0</v>
@@ -5504,7 +5499,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B113">
         <v>1</v>
@@ -5512,7 +5507,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B114">
         <v>1</v>
@@ -5520,7 +5515,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B115">
         <v>0</v>
@@ -5528,7 +5523,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B116">
         <v>0</v>
@@ -5536,7 +5531,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B117">
         <v>0</v>
@@ -5544,7 +5539,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B118">
         <v>0</v>
@@ -5552,7 +5547,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B119">
         <v>1</v>
@@ -5560,7 +5555,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B120">
         <v>1</v>
@@ -5568,7 +5563,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B121">
         <v>0</v>
@@ -5576,7 +5571,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B122">
         <v>0</v>
@@ -5584,7 +5579,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B123">
         <v>1</v>
@@ -5592,7 +5587,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B124">
         <v>1</v>
@@ -5600,7 +5595,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B125">
         <v>1</v>
@@ -5608,7 +5603,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B126">
         <v>1</v>
@@ -5616,7 +5611,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B127">
         <v>1</v>
@@ -5624,7 +5619,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B128">
         <v>1</v>
@@ -5632,7 +5627,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B129">
         <v>1</v>
@@ -5640,7 +5635,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B130">
         <v>1</v>
@@ -5648,7 +5643,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B131">
         <v>1</v>
@@ -5656,7 +5651,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B132">
         <v>1</v>
@@ -5664,7 +5659,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B133">
         <v>0</v>
@@ -5672,7 +5667,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B134">
         <v>0</v>
@@ -5680,7 +5675,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B135">
         <v>0</v>
@@ -5688,7 +5683,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B136">
         <v>0</v>
@@ -5696,7 +5691,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B137">
         <v>0</v>
@@ -5704,7 +5699,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B138">
         <v>1</v>
@@ -5712,7 +5707,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B139">
         <v>0</v>
@@ -5720,7 +5715,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B140">
         <v>0</v>
@@ -5728,7 +5723,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B141">
         <v>1</v>
@@ -5736,7 +5731,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B142">
         <v>0</v>
@@ -5744,7 +5739,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B143">
         <v>0</v>
@@ -5752,7 +5747,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B144">
         <v>1</v>
@@ -5760,7 +5755,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B145">
         <v>1</v>
@@ -5768,7 +5763,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B146">
         <v>0</v>
@@ -5776,7 +5771,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B147">
         <v>0</v>
@@ -5784,7 +5779,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B148">
         <v>0</v>
@@ -5792,7 +5787,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B149">
         <v>1</v>
@@ -5800,7 +5795,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B150">
         <v>0</v>
@@ -5808,7 +5803,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B151">
         <v>1</v>
@@ -5816,7 +5811,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B152">
         <v>1</v>
@@ -5824,7 +5819,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B153">
         <v>1</v>
@@ -5832,7 +5827,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B154">
         <v>1</v>
@@ -5840,7 +5835,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B155">
         <v>1</v>
@@ -5848,7 +5843,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B156">
         <v>0</v>
@@ -5856,7 +5851,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B157">
         <v>1</v>
@@ -5864,7 +5859,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B158">
         <v>1</v>
@@ -5872,7 +5867,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B159">
         <v>0</v>
@@ -5880,7 +5875,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B160">
         <v>0</v>
@@ -5888,7 +5883,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B161">
         <v>1</v>
@@ -5896,7 +5891,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B162">
         <v>0</v>
@@ -5904,7 +5899,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B163">
         <v>1</v>
@@ -5912,7 +5907,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B164">
         <v>1</v>
@@ -5920,7 +5915,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B165">
         <v>0</v>
@@ -5928,7 +5923,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B166">
         <v>1</v>
@@ -5936,7 +5931,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B167">
         <v>1</v>
@@ -5944,7 +5939,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B168">
         <v>1</v>
@@ -5952,7 +5947,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B169">
         <v>1</v>
@@ -5960,7 +5955,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B170">
         <v>1</v>
@@ -5968,7 +5963,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B171">
         <v>0</v>
@@ -5976,7 +5971,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B172">
         <v>1</v>
@@ -5984,7 +5979,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B173">
         <v>0</v>
@@ -5992,7 +5987,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B174">
         <v>1</v>
@@ -6000,7 +5995,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B175">
         <v>1</v>
@@ -6008,7 +6003,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B176">
         <v>0</v>
@@ -6016,7 +6011,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B177">
         <v>0</v>
@@ -6024,7 +6019,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B178">
         <v>1</v>
@@ -6032,7 +6027,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B179">
         <v>1</v>
@@ -6040,7 +6035,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B180">
         <v>1</v>
@@ -6048,7 +6043,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B181">
         <v>0</v>
@@ -6056,7 +6051,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B182">
         <v>0</v>
@@ -6064,7 +6059,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B183">
         <v>1</v>
@@ -6072,7 +6067,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B184">
         <v>1</v>
@@ -6080,7 +6075,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B185">
         <v>0</v>
@@ -6088,7 +6083,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B186">
         <v>1</v>
@@ -6096,7 +6091,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B187">
         <v>0</v>
@@ -6104,7 +6099,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B188">
         <v>1</v>
@@ -6112,7 +6107,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B189">
         <v>1</v>
@@ -6120,7 +6115,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B190">
         <v>1</v>
@@ -6128,7 +6123,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B191">
         <v>0</v>
@@ -6136,7 +6131,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B192">
         <v>0</v>
@@ -6144,7 +6139,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B193">
         <v>0</v>
@@ -6152,7 +6147,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B194">
         <v>1</v>
@@ -6160,7 +6155,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B195">
         <v>1</v>
@@ -6168,7 +6163,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B196">
         <v>1</v>
@@ -6176,7 +6171,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B197">
         <v>1</v>
@@ -6184,7 +6179,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B198">
         <v>0</v>
@@ -6192,7 +6187,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B199">
         <v>1</v>
@@ -6200,7 +6195,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B200">
         <v>1</v>
@@ -6208,7 +6203,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B201">
         <v>1</v>
@@ -6225,6 +6220,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008270B9C3304188429EFDB2E507900750" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f301f43fce1caed4b4c29696bd6d795f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="39b056dd-27ae-4f38-bd74-ea825229b6ba" xmlns:ns4="f06a68fc-ed8b-47cc-b084-1990e39abd28" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8d0b35255871ffd93df7f8b061f88664" ns3:_="" ns4:_="">
     <xsd:import namespace="39b056dd-27ae-4f38-bd74-ea825229b6ba"/>
@@ -6427,22 +6437,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C843C7F-43DB-4AA0-8FBD-7A36E60EDFE5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f06a68fc-ed8b-47cc-b084-1990e39abd28"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="39b056dd-27ae-4f38-bd74-ea825229b6ba"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9EAC86-3103-494F-B96C-9CB7ED461EF6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A42CD2EA-4674-4997-9B14-B7E1C0290972}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6459,29 +6479,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9EAC86-3103-494F-B96C-9CB7ED461EF6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C843C7F-43DB-4AA0-8FBD-7A36E60EDFE5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f06a68fc-ed8b-47cc-b084-1990e39abd28"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="39b056dd-27ae-4f38-bd74-ea825229b6ba"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>